<commit_message>
[IMP] Add partner detail report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_partner_list.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_partner_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t xml:space="preserve">Partner Category</t>
   </si>
@@ -115,13 +115,28 @@
     <t xml:space="preserve">Account Owner name</t>
   </si>
   <si>
-    <t xml:space="preserve">Activie</t>
+    <t xml:space="preserve">Active</t>
   </si>
   <si>
     <t xml:space="preserve">Default</t>
   </si>
   <si>
     <t xml:space="preserve">Income Tax Form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create By</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update By</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active/Inactive</t>
   </si>
 </sst>
 </file>
@@ -132,7 +147,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -168,8 +183,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +208,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFFF"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC2E0AE"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -238,7 +266,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -273,6 +301,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -284,6 +316,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFC2E0AE"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -292,10 +384,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AK5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AD11" activeCellId="0" sqref="AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -304,7 +396,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="6" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="1" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="27" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="37" style="0" width="17.4"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -436,6 +533,21 @@
       <c r="AF5" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="AG5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK5" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>

</xml_diff>